<commit_message>
corrected RNA isolation date
</commit_message>
<xml_diff>
--- a/s1cDNASample/s1CDNASample_J.PLAGGENBERG_10.12.20.xlsx
+++ b/s1cDNASample/s1CDNASample_J.PLAGGENBERG_10.12.20.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/s1cDNASample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2543D066-9115-6641-8474-EAA8236A2546}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA056DD-9B59-4B43-9D89-FD34FCF1F1C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13300" yWindow="460" windowWidth="20300" windowHeight="18780" xr2:uid="{FDFE8680-0327-0F4B-86FB-33A18ED5D85B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="17">
   <si>
     <t>rnaDate</t>
   </si>
@@ -57,9 +57,6 @@
     <t>s1PrimerSeq</t>
   </si>
   <si>
-    <t>09.25.20</t>
-  </si>
-  <si>
     <t>H.BROWN</t>
   </si>
   <si>
@@ -78,10 +75,7 @@
     <t>random</t>
   </si>
   <si>
-    <t>10.03.21</t>
-  </si>
-  <si>
-    <t>10.03.22</t>
+    <t>10.03.20</t>
   </si>
 </sst>
 </file>
@@ -436,7 +430,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C27"/>
+      <selection activeCell="A3" sqref="A3:A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -475,834 +469,834 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I2" t="b">
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I3" t="b">
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4">
         <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I4" t="b">
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5">
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I5" t="b">
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6">
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I6" t="b">
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F7">
         <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I7" t="b">
         <v>0</v>
       </c>
       <c r="J7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8">
         <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8">
         <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I8" t="b">
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F9">
         <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I9" t="b">
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F10">
         <v>9</v>
       </c>
       <c r="G10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I10" t="b">
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11">
         <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I11" t="b">
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12">
         <v>37</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F12">
         <v>11</v>
       </c>
       <c r="G12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I12" t="b">
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13">
         <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F13">
         <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I13" t="b">
         <v>0</v>
       </c>
       <c r="J13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14">
         <v>39</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14">
         <v>13</v>
       </c>
       <c r="G14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I14" t="b">
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15">
         <v>40</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15">
         <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I15" t="b">
         <v>0</v>
       </c>
       <c r="J15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C16">
         <v>41</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F16">
         <v>15</v>
       </c>
       <c r="G16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I16" t="b">
         <v>0</v>
       </c>
       <c r="J16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17">
         <v>42</v>
       </c>
       <c r="D17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F17">
         <v>16</v>
       </c>
       <c r="G17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I17" t="b">
         <v>0</v>
       </c>
       <c r="J17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18">
         <v>43</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F18">
         <v>17</v>
       </c>
       <c r="G18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I18" t="b">
         <v>0</v>
       </c>
       <c r="J18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C19">
         <v>44</v>
       </c>
       <c r="D19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F19">
         <v>18</v>
       </c>
       <c r="G19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I19" t="b">
         <v>0</v>
       </c>
       <c r="J19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20">
         <v>45</v>
       </c>
       <c r="D20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F20">
         <v>19</v>
       </c>
       <c r="G20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I20" t="b">
         <v>0</v>
       </c>
       <c r="J20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C21">
         <v>46</v>
       </c>
       <c r="D21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F21">
         <v>20</v>
       </c>
       <c r="G21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I21" t="b">
         <v>0</v>
       </c>
       <c r="J21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C22">
         <v>47</v>
       </c>
       <c r="D22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F22">
         <v>21</v>
       </c>
       <c r="G22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I22" t="b">
         <v>0</v>
       </c>
       <c r="J22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C23">
         <v>48</v>
       </c>
       <c r="D23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F23">
         <v>22</v>
       </c>
       <c r="G23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I23" t="b">
         <v>0</v>
       </c>
       <c r="J23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C24">
         <v>49</v>
       </c>
       <c r="D24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F24">
         <v>23</v>
       </c>
       <c r="G24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I24" t="b">
         <v>0</v>
       </c>
       <c r="J24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C25">
         <v>50</v>
       </c>
       <c r="D25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F25">
         <v>24</v>
       </c>
       <c r="G25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I25" t="b">
         <v>0</v>
       </c>
       <c r="J25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C26">
         <v>51</v>
       </c>
       <c r="D26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F26">
         <v>25</v>
       </c>
       <c r="G26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I26" t="b">
         <v>0</v>
       </c>
       <c r="J26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C27">
         <v>52</v>
       </c>
       <c r="D27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F27">
         <v>26</v>
       </c>
       <c r="G27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I27" t="b">
         <v>0</v>
       </c>
       <c r="J27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>